<commit_message>
temp fix to pagbsc to fix error, update fopity so start year is 2023
</commit_message>
<xml_diff>
--- a/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
+++ b/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shelley\Dropbox (Energy Innovation)\PC (2)\Documents\GitHub_Repositories\eps-california\InputData\elec\GBSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\California\CA-eps\InputData\elec\GBSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C0D297-4C3A-46D4-98EB-997F5E5EE7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B48268A-6A5A-498D-805C-E91D75071103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15345" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{45074998-618E-48D2-8BA8-70A9753ED4B7}"/>
+    <workbookView xWindow="1580" yWindow="620" windowWidth="19520" windowHeight="10130" activeTab="5" xr2:uid="{45074998-618E-48D2-8BA8-70A9753ED4B7}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -3230,7 +3230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
@@ -29658,8 +29658,8 @@
   </sheetPr>
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -29775,132 +29775,100 @@
         <v>124</v>
       </c>
       <c r="B2" s="17">
-        <f>BGBSC!B2</f>
-        <v>252.5</v>
+        <v>0</v>
       </c>
       <c r="C2" s="17">
-        <f>BGBSC!C2</f>
-        <v>524.29999999999995</v>
+        <v>0</v>
       </c>
       <c r="D2" s="17">
-        <f>BGBSC!D2</f>
-        <v>2842.27</v>
+        <v>0</v>
       </c>
       <c r="E2" s="17">
-        <f>BGBSC!E2</f>
-        <v>5160.24</v>
+        <v>0</v>
       </c>
       <c r="F2" s="17">
-        <f>BGBSC!F2</f>
-        <v>7563.37</v>
+        <v>0</v>
       </c>
       <c r="G2" s="17">
-        <f>BGBSC!G2</f>
-        <v>13055.18</v>
+        <v>0</v>
       </c>
       <c r="H2" s="17">
-        <f>BGBSC!H2</f>
-        <v>14769.37</v>
+        <v>0</v>
       </c>
       <c r="I2" s="17">
-        <f>BGBSC!I2</f>
-        <v>14983.48</v>
+        <v>0</v>
       </c>
       <c r="J2" s="17">
-        <f>BGBSC!J2</f>
-        <v>15585.665000000037</v>
+        <v>0</v>
       </c>
       <c r="K2" s="17">
-        <f>BGBSC!K2</f>
-        <v>16187.849999999999</v>
+        <v>0</v>
       </c>
       <c r="L2" s="17">
-        <f>BGBSC!L2</f>
-        <v>16576.844999999972</v>
+        <v>0</v>
       </c>
       <c r="M2" s="17">
-        <f>BGBSC!M2</f>
-        <v>16965.84</v>
+        <v>0</v>
       </c>
       <c r="N2" s="17">
-        <f>BGBSC!N2</f>
-        <v>17553.909999999916</v>
+        <v>0</v>
       </c>
       <c r="O2" s="17">
-        <f>BGBSC!O2</f>
-        <v>18141.98</v>
+        <v>0</v>
       </c>
       <c r="P2" s="17">
-        <f>BGBSC!P2</f>
-        <v>19501.040000000037</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="17">
-        <f>BGBSC!Q2</f>
-        <v>20860.100000000093</v>
+        <v>0</v>
       </c>
       <c r="R2" s="17">
-        <f>BGBSC!R2</f>
-        <v>22219.159999999996</v>
+        <v>0</v>
       </c>
       <c r="S2" s="17">
-        <f>BGBSC!S2</f>
-        <v>24395.25800000038</v>
+        <v>0</v>
       </c>
       <c r="T2" s="17">
-        <f>BGBSC!T2</f>
-        <v>26571.356000000611</v>
+        <v>0</v>
       </c>
       <c r="U2" s="17">
-        <f>BGBSC!U2</f>
-        <v>28747.453999999911</v>
+        <v>0</v>
       </c>
       <c r="V2" s="17">
-        <f>BGBSC!V2</f>
-        <v>30923.552000000142</v>
+        <v>0</v>
       </c>
       <c r="W2" s="17">
-        <f>BGBSC!W2</f>
-        <v>33099.650000000373</v>
+        <v>0</v>
       </c>
       <c r="X2" s="17">
-        <f>BGBSC!X2</f>
-        <v>35535.195999999531</v>
+        <v>0</v>
       </c>
       <c r="Y2" s="17">
-        <f>BGBSC!Y2</f>
-        <v>37970.74199999962</v>
+        <v>0</v>
       </c>
       <c r="Z2" s="17">
-        <f>BGBSC!Z2</f>
-        <v>40406.287999998778</v>
+        <v>0</v>
       </c>
       <c r="AA2" s="17">
-        <f>BGBSC!AA2</f>
-        <v>42841.833999998868</v>
+        <v>0</v>
       </c>
       <c r="AB2" s="17">
-        <f>BGBSC!AB2</f>
-        <v>45277.379999998957</v>
+        <v>0</v>
       </c>
       <c r="AC2" s="17">
-        <f>BGBSC!AC2</f>
-        <v>47712.925999999046</v>
+        <v>0</v>
       </c>
       <c r="AD2" s="17">
-        <f>BGBSC!AD2</f>
-        <v>50148.471999999136</v>
+        <v>0</v>
       </c>
       <c r="AE2" s="17">
-        <f>BGBSC!AE2</f>
-        <v>52584.017999999225</v>
+        <v>0</v>
       </c>
       <c r="AF2" s="17">
-        <f>BGBSC!AF2</f>
-        <v>55019.563999999315</v>
+        <v>0</v>
       </c>
       <c r="AG2" s="17">
-        <f>BGBSC!AG2</f>
-        <v>57455.109999999404</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated elec/GBSC for potential added grid battery storage capacity and updates to webappdata policy descriptions
</commit_message>
<xml_diff>
--- a/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
+++ b/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\California\CA-eps\InputData\elec\GBSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shelley\Dropbox (Energy Innovation)\PC (2)\Documents\GitHub_Repositories\eps-california\InputData\elec\GBSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B48268A-6A5A-498D-805C-E91D75071103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42339C7F-E410-4993-8366-891977A22E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="620" windowWidth="19520" windowHeight="10130" activeTab="5" xr2:uid="{45074998-618E-48D2-8BA8-70A9753ED4B7}"/>
+    <workbookView xWindow="15345" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{45074998-618E-48D2-8BA8-70A9753ED4B7}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -29401,7 +29401,7 @@
   </sheetPr>
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
@@ -29659,7 +29659,7 @@
   <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -29775,100 +29775,132 @@
         <v>124</v>
       </c>
       <c r="B2" s="17">
-        <v>0</v>
+        <f>BGBSC!B2</f>
+        <v>252.5</v>
       </c>
       <c r="C2" s="17">
-        <v>0</v>
+        <f>BGBSC!C2</f>
+        <v>524.29999999999995</v>
       </c>
       <c r="D2" s="17">
-        <v>0</v>
+        <f>BGBSC!D2</f>
+        <v>2842.27</v>
       </c>
       <c r="E2" s="17">
-        <v>0</v>
+        <f>BGBSC!E2</f>
+        <v>5160.24</v>
       </c>
       <c r="F2" s="17">
-        <v>0</v>
+        <f>BGBSC!F2</f>
+        <v>7563.37</v>
       </c>
       <c r="G2" s="17">
-        <v>0</v>
+        <f>BGBSC!G2</f>
+        <v>13055.18</v>
       </c>
       <c r="H2" s="17">
-        <v>0</v>
+        <f>BGBSC!H2</f>
+        <v>14769.37</v>
       </c>
       <c r="I2" s="17">
-        <v>0</v>
+        <f>BGBSC!I2</f>
+        <v>14983.48</v>
       </c>
       <c r="J2" s="17">
-        <v>0</v>
+        <f>BGBSC!J2</f>
+        <v>15585.665000000037</v>
       </c>
       <c r="K2" s="17">
-        <v>0</v>
+        <f>BGBSC!K2</f>
+        <v>16187.849999999999</v>
       </c>
       <c r="L2" s="17">
-        <v>0</v>
+        <f>BGBSC!L2</f>
+        <v>16576.844999999972</v>
       </c>
       <c r="M2" s="17">
-        <v>0</v>
+        <f>BGBSC!M2</f>
+        <v>16965.84</v>
       </c>
       <c r="N2" s="17">
-        <v>0</v>
+        <f>BGBSC!N2</f>
+        <v>17553.909999999916</v>
       </c>
       <c r="O2" s="17">
-        <v>0</v>
+        <f>BGBSC!O2</f>
+        <v>18141.98</v>
       </c>
       <c r="P2" s="17">
-        <v>0</v>
+        <f>BGBSC!P2</f>
+        <v>19501.040000000037</v>
       </c>
       <c r="Q2" s="17">
-        <v>0</v>
+        <f>BGBSC!Q2</f>
+        <v>20860.100000000093</v>
       </c>
       <c r="R2" s="17">
-        <v>0</v>
+        <f>BGBSC!R2</f>
+        <v>22219.159999999996</v>
       </c>
       <c r="S2" s="17">
-        <v>0</v>
+        <f>BGBSC!S2</f>
+        <v>24395.25800000038</v>
       </c>
       <c r="T2" s="17">
-        <v>0</v>
+        <f>BGBSC!T2</f>
+        <v>26571.356000000611</v>
       </c>
       <c r="U2" s="17">
-        <v>0</v>
+        <f>BGBSC!U2</f>
+        <v>28747.453999999911</v>
       </c>
       <c r="V2" s="17">
-        <v>0</v>
+        <f>BGBSC!V2</f>
+        <v>30923.552000000142</v>
       </c>
       <c r="W2" s="17">
-        <v>0</v>
+        <f>BGBSC!W2</f>
+        <v>33099.650000000373</v>
       </c>
       <c r="X2" s="17">
-        <v>0</v>
+        <f>BGBSC!X2</f>
+        <v>35535.195999999531</v>
       </c>
       <c r="Y2" s="17">
-        <v>0</v>
+        <f>BGBSC!Y2</f>
+        <v>37970.74199999962</v>
       </c>
       <c r="Z2" s="17">
-        <v>0</v>
+        <f>BGBSC!Z2</f>
+        <v>40406.287999998778</v>
       </c>
       <c r="AA2" s="17">
-        <v>0</v>
+        <f>BGBSC!AA2</f>
+        <v>42841.833999998868</v>
       </c>
       <c r="AB2" s="17">
-        <v>0</v>
+        <f>BGBSC!AB2</f>
+        <v>45277.379999998957</v>
       </c>
       <c r="AC2" s="17">
-        <v>0</v>
+        <f>BGBSC!AC2</f>
+        <v>47712.925999999046</v>
       </c>
       <c r="AD2" s="17">
-        <v>0</v>
+        <f>BGBSC!AD2</f>
+        <v>50148.471999999136</v>
       </c>
       <c r="AE2" s="17">
-        <v>0</v>
+        <f>BGBSC!AE2</f>
+        <v>52584.017999999225</v>
       </c>
       <c r="AF2" s="17">
-        <v>0</v>
+        <f>BGBSC!AF2</f>
+        <v>55019.563999999315</v>
       </c>
       <c r="AG2" s="17">
-        <v>0</v>
+        <f>BGBSC!AG2</f>
+        <v>57455.109999999404</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to storage capacities and policy schedule for storage deployment
</commit_message>
<xml_diff>
--- a/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
+++ b/InputData/elec/GBSC/Grid Battery Storage Capacities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shelley\Dropbox (Energy Innovation)\PC (2)\Documents\GitHub_Repositories\eps-california\InputData\elec\GBSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\California\Models\eps-california\InputData\elec\GBSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42339C7F-E410-4993-8366-891977A22E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37E0B04-1B98-4408-B887-6EFC30A732BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15345" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{45074998-618E-48D2-8BA8-70A9753ED4B7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="5" xr2:uid="{45074998-618E-48D2-8BA8-70A9753ED4B7}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -3234,15 +3234,15 @@
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" style="6" customWidth="1"/>
     <col min="2" max="2" width="54" style="6" customWidth="1"/>
     <col min="3" max="3" width="9" style="6" customWidth="1"/>
     <col min="4" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F4" s="8" t="s">
         <v>10</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -3318,7 +3318,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>2020</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>20</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>26</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F11" s="8" t="s">
         <v>29</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>34</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>37</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>40</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>43</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>46</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
       <c r="F18" s="8" t="s">
         <v>49</v>
@@ -3445,7 +3445,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>51</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>15</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
         <v>2018</v>
       </c>
@@ -3478,7 +3478,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>58</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>26</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="F25" s="8" t="s">
         <v>65</v>
@@ -3520,7 +3520,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>127</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>131</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>128</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>130</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>129</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F31" s="8" t="s">
         <v>81</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>289</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>131</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="6" t="s">
         <v>128</v>
@@ -3617,7 +3617,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="6" t="s">
         <v>129</v>
@@ -3629,7 +3629,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" s="6">
         <v>2021</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F37" s="8" t="s">
         <v>93</v>
       </c>
@@ -3648,7 +3648,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F38" s="8" t="s">
         <v>95</v>
       </c>
@@ -3656,7 +3656,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F39" s="8" t="s">
         <v>97</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>67</v>
       </c>
@@ -3675,7 +3675,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -3686,7 +3686,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>73</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F43" s="8" t="s">
         <v>105</v>
       </c>
@@ -3705,7 +3705,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>78</v>
       </c>
@@ -3716,7 +3716,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>355</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F46" s="8" t="s">
         <v>111</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F47" s="8" t="s">
         <v>113</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F48" s="8" t="s">
         <v>115</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F49" s="8" t="s">
         <v>117</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="50" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F50" s="8" t="s">
         <v>119</v>
       </c>
@@ -3785,37 +3785,37 @@
   </sheetPr>
   <dimension ref="B2:AK224"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M99" sqref="M99:AK99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.08984375" customWidth="1"/>
-    <col min="3" max="3" width="24.1796875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="15.81640625" customWidth="1"/>
-    <col min="14" max="15" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.26953125" customWidth="1"/>
-    <col min="20" max="20" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.26953125" customWidth="1"/>
-    <col min="22" max="22" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.26953125" customWidth="1"/>
-    <col min="24" max="24" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="9.26953125" customWidth="1"/>
-    <col min="27" max="27" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="31" width="9.26953125" customWidth="1"/>
-    <col min="32" max="32" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="33" max="36" width="9.26953125" customWidth="1"/>
-    <col min="37" max="37" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="14" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.28515625" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.28515625" customWidth="1"/>
+    <col min="24" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="9.28515625" customWidth="1"/>
+    <col min="27" max="27" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="31" width="9.28515625" customWidth="1"/>
+    <col min="32" max="32" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="36" width="9.28515625" customWidth="1"/>
+    <col min="37" max="37" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
         <v>134</v>
       </c>
@@ -3823,10 +3823,10 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
         <v>135</v>
@@ -3835,7 +3835,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
         <v>137</v>
@@ -3847,7 +3847,7 @@
         <v>840383.03557274048</v>
       </c>
     </row>
-    <row r="8" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
         <v>139</v>
@@ -3859,7 +3859,7 @@
         <v>903514.35131486552</v>
       </c>
     </row>
-    <row r="9" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" s="6" t="s">
         <v>140</v>
@@ -3871,7 +3871,7 @@
         <v>45313.653841965206</v>
       </c>
     </row>
-    <row r="10" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
         <v>141</v>
@@ -3883,7 +3883,7 @@
         <v>48717.709453555246</v>
       </c>
     </row>
-    <row r="11" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
         <v>142</v>
@@ -3895,10 +3895,10 @@
         <v>19.571024255801614</v>
       </c>
     </row>
-    <row r="12" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="C13" s="6" t="s">
         <v>144</v>
@@ -4000,7 +4000,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="14" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="6" t="s">
         <v>145</v>
@@ -4102,7 +4102,7 @@
         <v>54786.831366782942</v>
       </c>
     </row>
-    <row r="15" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="6" t="s">
         <v>147</v>
@@ -4204,7 +4204,7 @@
         <v>59169.545356248542</v>
       </c>
     </row>
-    <row r="16" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
         <v>148</v>
@@ -4306,7 +4306,7 @@
         <v>20.164213098037326</v>
       </c>
     </row>
-    <row r="17" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="C17" s="6" t="s">
         <v>149</v>
@@ -4408,7 +4408,7 @@
         <v>12.251380089769448</v>
       </c>
     </row>
-    <row r="18" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
         <v>151</v>
@@ -4510,7 +4510,7 @@
         <v>0.97081968260457008</v>
       </c>
     </row>
-    <row r="19" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="C19" s="6" t="s">
         <v>153</v>
@@ -4612,19 +4612,19 @@
         <v>0.20550868960983881</v>
       </c>
     </row>
-    <row r="20" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
     </row>
-    <row r="21" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="C21" s="6" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
     </row>
-    <row r="23" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="D23" t="s">
         <v>136</v>
@@ -4723,7 +4723,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="24" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="C24" s="6" t="s">
         <v>156</v>
@@ -4825,7 +4825,7 @@
         <v>926.0200000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
       <c r="C25" s="6" t="s">
         <v>158</v>
@@ -4927,7 +4927,7 @@
         <v>134.38999999999999</v>
       </c>
     </row>
-    <row r="26" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
       <c r="C26" s="6" t="s">
         <v>159</v>
@@ -5029,7 +5029,7 @@
         <v>1521.4099999999999</v>
       </c>
     </row>
-    <row r="27" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
       <c r="C27" s="6" t="s">
         <v>160</v>
@@ -5131,7 +5131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
       <c r="C28" s="6" t="s">
         <v>161</v>
@@ -5233,7 +5233,7 @@
         <v>5031.2700000000004</v>
       </c>
     </row>
-    <row r="29" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="C29" s="6" t="s">
         <v>162</v>
@@ -5335,7 +5335,7 @@
         <v>1970.2</v>
       </c>
     </row>
-    <row r="30" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
       <c r="C30" s="6" t="s">
         <v>163</v>
@@ -5437,7 +5437,7 @@
         <v>1728.08</v>
       </c>
     </row>
-    <row r="31" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
       <c r="C31" s="6" t="s">
         <v>164</v>
@@ -5539,7 +5539,7 @@
         <v>72340.25</v>
       </c>
     </row>
-    <row r="32" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="C32" s="6" t="s">
         <v>165</v>
@@ -5641,7 +5641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:37" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:37" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C33" s="29" t="s">
         <v>166</v>
       </c>
@@ -5743,7 +5743,7 @@
       </c>
       <c r="AK33" s="30"/>
     </row>
-    <row r="34" spans="2:37" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:37" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C34" s="29" t="s">
         <v>167</v>
       </c>
@@ -5844,7 +5844,7 @@
         <v>1000.28</v>
       </c>
     </row>
-    <row r="35" spans="2:37" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:37" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="29" t="s">
         <v>168</v>
       </c>
@@ -5945,7 +5945,7 @@
         <v>440.66</v>
       </c>
     </row>
-    <row r="36" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="C36" s="6" t="s">
         <v>169</v>
@@ -6047,7 +6047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B37" s="6"/>
       <c r="C37" s="6" t="s">
         <v>170</v>
@@ -6149,7 +6149,7 @@
         <v>42147.01</v>
       </c>
     </row>
-    <row r="38" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="C38" s="6" t="s">
         <v>171</v>
@@ -6251,10 +6251,10 @@
         <v>125798.63</v>
       </c>
     </row>
-    <row r="39" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
     </row>
-    <row r="40" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
       <c r="C40" s="6" t="s">
         <v>172</v>
@@ -6353,7 +6353,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="41" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B41" s="6"/>
       <c r="C41" s="6" t="s">
         <v>173</v>
@@ -6455,7 +6455,7 @@
         <v>12.000000000000002</v>
       </c>
     </row>
-    <row r="42" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="C42" s="6" t="s">
         <v>175</v>
@@ -6557,7 +6557,7 @@
         <v>7.8752872041649118</v>
       </c>
     </row>
-    <row r="43" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="C43" s="6" t="s">
         <v>176</v>
@@ -6659,7 +6659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
       <c r="C44" s="6" t="s">
         <v>177</v>
@@ -6761,25 +6761,25 @@
         <v>4.3846153846153841</v>
       </c>
     </row>
-    <row r="45" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
       <c r="C45" s="6" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="46" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B46" s="6"/>
     </row>
-    <row r="47" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B47" s="6"/>
       <c r="C47" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="48" spans="2:37" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
     </row>
-    <row r="49" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B49" s="6"/>
       <c r="D49" t="s">
         <v>136</v>
@@ -6878,7 +6878,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="50" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B50" s="6"/>
       <c r="C50" s="6" t="s">
         <v>180</v>
@@ -6980,7 +6980,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="51" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="C51" s="6" t="s">
         <v>181</v>
@@ -7082,7 +7082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B52" s="6"/>
       <c r="C52" s="6" t="s">
         <v>156</v>
@@ -7184,7 +7184,7 @@
         <v>25668.15</v>
       </c>
     </row>
-    <row r="53" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
       <c r="C53" s="6" t="s">
         <v>182</v>
@@ -7286,7 +7286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
       <c r="C54" s="6" t="s">
         <v>183</v>
@@ -7388,7 +7388,7 @@
         <v>7072.77</v>
       </c>
     </row>
-    <row r="55" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="C55" s="6" t="s">
         <v>184</v>
@@ -7490,7 +7490,7 @@
         <v>2851.77</v>
       </c>
     </row>
-    <row r="56" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B56" s="6"/>
       <c r="C56" s="6" t="s">
         <v>158</v>
@@ -7592,7 +7592,7 @@
         <v>942.11</v>
       </c>
     </row>
-    <row r="57" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
       <c r="C57" s="6" t="s">
         <v>159</v>
@@ -7694,7 +7694,7 @@
         <v>3108.85</v>
       </c>
     </row>
-    <row r="58" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B58" s="6"/>
       <c r="C58" s="6" t="s">
         <v>160</v>
@@ -7796,7 +7796,7 @@
         <v>958.32999999999993</v>
       </c>
     </row>
-    <row r="59" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B59" s="6"/>
       <c r="C59" s="6" t="s">
         <v>161</v>
@@ -7898,7 +7898,7 @@
         <v>12001.390000000001</v>
       </c>
     </row>
-    <row r="60" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B60" s="6"/>
       <c r="C60" s="6" t="s">
         <v>162</v>
@@ -8000,7 +8000,7 @@
         <v>1970.2</v>
       </c>
     </row>
-    <row r="61" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B61" s="6"/>
       <c r="C61" s="6" t="s">
         <v>163</v>
@@ -8102,7 +8102,7 @@
         <v>1728.08</v>
       </c>
     </row>
-    <row r="62" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B62" s="6"/>
       <c r="C62" s="6" t="s">
         <v>164</v>
@@ -8204,7 +8204,7 @@
         <v>88757.04</v>
       </c>
     </row>
-    <row r="63" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B63" s="6"/>
       <c r="C63" s="18" t="s">
         <v>165</v>
@@ -8306,7 +8306,7 @@
         <v>37373.519999999997</v>
       </c>
     </row>
-    <row r="64" spans="2:36" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C64" s="10" t="s">
         <v>166</v>
       </c>
@@ -8407,7 +8407,7 @@
         <v>45277.38</v>
       </c>
     </row>
-    <row r="65" spans="2:36" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:36" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C65" s="10" t="s">
         <v>167</v>
       </c>
@@ -8508,7 +8508,7 @@
         <v>2898.7799999999997</v>
       </c>
     </row>
-    <row r="66" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B66" s="6"/>
       <c r="C66" s="18" t="s">
         <v>168</v>
@@ -8610,7 +8610,7 @@
         <v>2636.1099999999997</v>
       </c>
     </row>
-    <row r="67" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B67" s="6"/>
       <c r="C67" s="18" t="s">
         <v>185</v>
@@ -8712,7 +8712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B68" s="6"/>
       <c r="C68" s="18" t="s">
         <v>186</v>
@@ -8814,7 +8814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B69" s="6"/>
       <c r="C69" s="18" t="s">
         <v>187</v>
@@ -8916,7 +8916,7 @@
         <v>0.80223071314605854</v>
       </c>
     </row>
-    <row r="70" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B70" s="6"/>
       <c r="C70" s="6" t="s">
         <v>189</v>
@@ -9018,7 +9018,7 @@
         <v>392.47</v>
       </c>
     </row>
-    <row r="71" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B71" s="6"/>
       <c r="C71" s="6" t="s">
         <v>190</v>
@@ -9120,7 +9120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B72" s="6"/>
       <c r="C72" s="6" t="s">
         <v>191</v>
@@ -9222,22 +9222,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B73" s="6"/>
     </row>
-    <row r="74" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B74" s="6"/>
     </row>
-    <row r="75" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B75" s="6"/>
       <c r="C75" s="6" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="76" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B76" s="6"/>
     </row>
-    <row r="77" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B77" s="6"/>
       <c r="D77" t="s">
         <v>136</v>
@@ -9336,7 +9336,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="78" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B78" s="6"/>
       <c r="C78" s="5" t="s">
         <v>181</v>
@@ -9438,7 +9438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B79" s="6"/>
       <c r="C79" s="5" t="s">
         <v>180</v>
@@ -9540,7 +9540,7 @@
         <v>5108.3689805718604</v>
       </c>
     </row>
-    <row r="80" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B80" s="6"/>
       <c r="C80" s="5" t="s">
         <v>194</v>
@@ -9642,7 +9642,7 @@
         <v>18704.195858741459</v>
       </c>
     </row>
-    <row r="81" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B81" s="6"/>
       <c r="C81" s="5" t="s">
         <v>184</v>
@@ -9744,7 +9744,7 @@
         <v>8318.7176689951302</v>
       </c>
     </row>
-    <row r="82" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B82" s="6"/>
       <c r="C82" s="5" t="s">
         <v>156</v>
@@ -9846,7 +9846,7 @@
         <v>27966.978210015666</v>
       </c>
     </row>
-    <row r="83" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B83" s="6"/>
       <c r="C83" s="5" t="s">
         <v>182</v>
@@ -9948,7 +9948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B84" s="6"/>
       <c r="C84" s="6" t="s">
         <v>195</v>
@@ -10050,7 +10050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B85" s="6"/>
       <c r="C85" s="4" t="s">
         <v>196</v>
@@ -10152,7 +10152,7 @@
         <v>346903.77582883823</v>
       </c>
     </row>
-    <row r="86" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B86" s="6"/>
       <c r="C86" s="4" t="s">
         <v>197</v>
@@ -10254,7 +10254,7 @@
         <v>-21270.880775694422</v>
       </c>
     </row>
-    <row r="87" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B87" s="6"/>
       <c r="C87" s="4" t="s">
         <v>198</v>
@@ -10356,7 +10356,7 @@
         <v>-42655.161285813389</v>
       </c>
     </row>
-    <row r="88" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B88" s="6"/>
       <c r="C88" s="6" t="s">
         <v>199</v>
@@ -10458,7 +10458,7 @@
         <v>3631.8028000397217</v>
       </c>
     </row>
-    <row r="89" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B89" s="6"/>
       <c r="C89" s="6" t="s">
         <v>200</v>
@@ -10560,7 +10560,7 @@
         <v>-21392.482888187973</v>
       </c>
     </row>
-    <row r="90" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B90" s="6"/>
       <c r="C90" s="6" t="s">
         <v>201</v>
@@ -10662,7 +10662,7 @@
         <v>363495.33868168597</v>
       </c>
     </row>
-    <row r="91" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B91" s="6"/>
       <c r="M91">
         <v>241.07272535884886</v>
@@ -10737,16 +10737,16 @@
         <v>346.7077972856942</v>
       </c>
     </row>
-    <row r="92" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B92" s="6"/>
       <c r="C92" s="6" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="93" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B93" s="6"/>
     </row>
-    <row r="94" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B94" s="6"/>
       <c r="C94" s="6" t="s">
         <v>203</v>
@@ -10848,7 +10848,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="95" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B95" s="6"/>
       <c r="C95" s="6" t="s">
         <v>204</v>
@@ -10950,7 +10950,7 @@
         <v>41674.235554620675</v>
       </c>
     </row>
-    <row r="96" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B96" s="6"/>
       <c r="C96" s="6" t="s">
         <v>205</v>
@@ -11052,7 +11052,7 @@
         <v>231.662297193466</v>
       </c>
     </row>
-    <row r="97" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B97" s="6"/>
       <c r="C97" s="6" t="s">
         <v>206</v>
@@ -11154,7 +11154,7 @@
         <v>320.91262108000001</v>
       </c>
     </row>
-    <row r="98" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B98" s="6"/>
       <c r="C98" s="6" t="s">
         <v>207</v>
@@ -11256,7 +11256,7 @@
         <v>6792.9459193200009</v>
       </c>
     </row>
-    <row r="99" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B99" s="6"/>
       <c r="C99" s="6" t="s">
         <v>208</v>
@@ -11358,7 +11358,7 @@
         <v>5383.1230530900002</v>
       </c>
     </row>
-    <row r="100" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B100" s="6"/>
       <c r="C100" s="6" t="s">
         <v>209</v>
@@ -11460,7 +11460,7 @@
         <v>97.24727141999999</v>
       </c>
     </row>
-    <row r="101" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B101" s="6"/>
       <c r="C101" s="6" t="s">
         <v>210</v>
@@ -11562,7 +11562,7 @@
         <v>35.774254130000003</v>
       </c>
     </row>
-    <row r="102" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B102" s="6"/>
       <c r="C102" s="6" t="s">
         <v>211</v>
@@ -11664,7 +11664,7 @@
         <v>304.94043123999995</v>
       </c>
     </row>
-    <row r="103" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B103" s="6"/>
       <c r="C103" s="6" t="s">
         <v>212</v>
@@ -11766,7 +11766,7 @@
         <v>-54.010035311197271</v>
       </c>
     </row>
-    <row r="104" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B104" s="6"/>
       <c r="C104" s="6" t="s">
         <v>213</v>
@@ -11868,7 +11868,7 @@
         <v>54786.831366782942</v>
       </c>
     </row>
-    <row r="105" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B105" s="6"/>
       <c r="C105" s="6" t="s">
         <v>214</v>
@@ -11970,7 +11970,7 @@
         <v>4382.7139894656002</v>
       </c>
     </row>
-    <row r="106" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B106" s="6"/>
       <c r="C106" s="6" t="s">
         <v>147</v>
@@ -12072,7 +12072,7 @@
         <v>59169.545356248542</v>
       </c>
     </row>
-    <row r="107" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B107" s="6"/>
       <c r="C107" s="6" t="s">
         <v>215</v>
@@ -12174,7 +12174,7 @@
         <v>271703.29484424856</v>
       </c>
     </row>
-    <row r="108" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B108" s="6"/>
       <c r="C108" s="6" t="s">
         <v>216</v>
@@ -12276,7 +12276,7 @@
         <v>20.164213098037326</v>
       </c>
     </row>
-    <row r="109" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B109" s="6"/>
       <c r="C109" s="6" t="s">
         <v>217</v>
@@ -12357,7 +12357,7 @@
         <v>21914.732546713178</v>
       </c>
     </row>
-    <row r="110" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B110" s="6"/>
       <c r="C110" s="6" t="s">
         <v>218</v>
@@ -12438,7 +12438,7 @@
         <v>76613.109578431104</v>
       </c>
     </row>
-    <row r="111" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B111" s="6"/>
       <c r="C111" s="6" t="s">
         <v>220</v>
@@ -12519,7 +12519,7 @@
         <v>0.28604415963926405</v>
       </c>
     </row>
-    <row r="112" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B112" s="6"/>
       <c r="C112" s="6" t="s">
         <v>222</v>
@@ -12600,7 +12600,7 @@
         <v>143.02207981963201</v>
       </c>
     </row>
-    <row r="113" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B113" s="6"/>
       <c r="C113" s="6" t="s">
         <v>224</v>
@@ -12681,10 +12681,10 @@
         <v>171.62649578355843</v>
       </c>
     </row>
-    <row r="114" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B114" s="6"/>
     </row>
-    <row r="115" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B115" s="6"/>
       <c r="C115" s="6" t="s">
         <v>225</v>
@@ -12786,7 +12786,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="116" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B116" s="6"/>
       <c r="C116" s="6" t="s">
         <v>226</v>
@@ -12888,7 +12888,7 @@
         <v>1725.1822356955181</v>
       </c>
     </row>
-    <row r="117" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B117" s="6"/>
       <c r="C117" s="6" t="s">
         <v>227</v>
@@ -12990,7 +12990,7 @@
         <v>203.21735969038855</v>
       </c>
     </row>
-    <row r="118" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B118" s="6"/>
       <c r="C118" s="6" t="s">
         <v>228</v>
@@ -13092,7 +13092,7 @@
         <v>-734.44180527012122</v>
       </c>
     </row>
-    <row r="119" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B119" s="6"/>
       <c r="C119" s="6" t="s">
         <v>229</v>
@@ -13194,7 +13194,7 @@
         <v>-1247.9678254269827</v>
       </c>
     </row>
-    <row r="120" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B120" s="6"/>
       <c r="C120" s="6" t="s">
         <v>230</v>
@@ -13296,19 +13296,19 @@
         <v>-54.010035311197271</v>
       </c>
     </row>
-    <row r="121" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B121" s="6"/>
     </row>
-    <row r="122" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B122" s="6"/>
       <c r="C122" s="6" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="123" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B123" s="6"/>
     </row>
-    <row r="124" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B124" s="6"/>
       <c r="D124" t="s">
         <v>136</v>
@@ -13407,7 +13407,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="125" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B125" s="6"/>
       <c r="C125" s="6" t="s">
         <v>232</v>
@@ -13509,7 +13509,7 @@
         <v>0.87291531979507586</v>
       </c>
     </row>
-    <row r="126" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B126" s="6"/>
       <c r="C126" s="6" t="s">
         <v>233</v>
@@ -13611,7 +13611,7 @@
         <v>0.97081968260457008</v>
       </c>
     </row>
-    <row r="127" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B127" s="6"/>
       <c r="C127" s="6" t="s">
         <v>234</v>
@@ -13713,7 +13713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B128" s="6"/>
       <c r="C128" s="6" t="s">
         <v>235</v>
@@ -13815,7 +13815,7 @@
         <v>0.97081968260457008</v>
       </c>
     </row>
-    <row r="129" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B129" s="6"/>
       <c r="C129" s="6" t="s">
         <v>236</v>
@@ -13917,7 +13917,7 @@
         <v>0.13606641803746672</v>
       </c>
     </row>
-    <row r="130" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B130" s="6"/>
       <c r="C130" s="6" t="s">
         <v>153</v>
@@ -14019,7 +14019,7 @@
         <v>0.20550868960983881</v>
       </c>
     </row>
-    <row r="131" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B131" s="6"/>
       <c r="C131" s="6" t="s">
         <v>237</v>
@@ -14121,7 +14121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B132" s="6"/>
       <c r="C132" s="6" t="s">
         <v>239</v>
@@ -14223,7 +14223,7 @@
         <v>279227.4339611684</v>
       </c>
     </row>
-    <row r="133" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B133" s="6"/>
       <c r="C133" s="6" t="s">
         <v>240</v>
@@ -14325,7 +14325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B134" s="6"/>
       <c r="C134" s="6" t="s">
         <v>241</v>
@@ -14427,7 +14427,7 @@
         <v>1307.9556</v>
       </c>
     </row>
-    <row r="135" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B135" s="6"/>
       <c r="C135" s="6" t="s">
         <v>242</v>
@@ -14529,25 +14529,25 @@
         <v>1.0588148679987655</v>
       </c>
     </row>
-    <row r="136" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B136" s="6"/>
     </row>
-    <row r="137" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B137" s="6"/>
     </row>
-    <row r="138" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B138" s="6"/>
     </row>
-    <row r="139" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B139" s="6"/>
       <c r="C139" s="6" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="140" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B140" s="6"/>
     </row>
-    <row r="141" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B141" s="6"/>
       <c r="D141" t="s">
         <v>136</v>
@@ -14646,7 +14646,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="142" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B142" s="6"/>
       <c r="C142" s="6" t="s">
         <v>244</v>
@@ -14748,7 +14748,7 @@
         <v>12.25146299</v>
       </c>
     </row>
-    <row r="143" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B143" s="6"/>
       <c r="C143" s="6" t="s">
         <v>245</v>
@@ -14850,7 +14850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B144" s="6"/>
       <c r="C144" s="6" t="s">
         <v>246</v>
@@ -14952,7 +14952,7 @@
         <v>12.25146299</v>
       </c>
     </row>
-    <row r="145" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B145" s="6"/>
       <c r="C145" s="6" t="s">
         <v>247</v>
@@ -15054,7 +15054,7 @@
         <v>10.696979733542037</v>
       </c>
     </row>
-    <row r="146" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B146" s="6"/>
       <c r="C146" s="6" t="s">
         <v>248</v>
@@ -15156,7 +15156,7 @@
         <v>1.5544003562274107</v>
       </c>
     </row>
-    <row r="147" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B147" s="6"/>
       <c r="C147" s="6" t="s">
         <v>249</v>
@@ -15258,7 +15258,7 @@
         <v>12.251380089769448</v>
       </c>
     </row>
-    <row r="148" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B148" s="6"/>
       <c r="C148" s="6" t="s">
         <v>250</v>
@@ -15360,7 +15360,7 @@
         <v>269.38</v>
       </c>
     </row>
-    <row r="149" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B149" s="6"/>
       <c r="C149" s="6" t="s">
         <v>252</v>
@@ -15462,7 +15462,7 @@
         <v>60.600734945964597</v>
       </c>
     </row>
-    <row r="150" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B150" s="6"/>
       <c r="C150" s="6" t="s">
         <v>253</v>
@@ -15564,10 +15564,10 @@
         <v>329.98073494596457</v>
       </c>
     </row>
-    <row r="151" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B151" s="6"/>
     </row>
-    <row r="152" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B152" s="6"/>
       <c r="C152" s="6" t="s">
         <v>254</v>
@@ -15669,31 +15669,31 @@
         <v>142.3868184597317</v>
       </c>
     </row>
-    <row r="153" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B153" s="6"/>
     </row>
-    <row r="154" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B154" s="6"/>
     </row>
-    <row r="155" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B155" s="6"/>
     </row>
-    <row r="156" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B156" s="6"/>
     </row>
-    <row r="157" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B157" s="6"/>
     </row>
-    <row r="158" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B158" s="6"/>
       <c r="C158" s="6" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="159" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B159" s="6"/>
     </row>
-    <row r="160" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B160" s="6"/>
       <c r="D160" t="s">
         <v>136</v>
@@ -15792,7 +15792,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="161" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B161" s="6"/>
       <c r="C161" s="6" t="s">
         <v>256</v>
@@ -15894,7 +15894,7 @@
         <v>56439.35</v>
       </c>
     </row>
-    <row r="162" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B162" s="6"/>
       <c r="C162" s="6" t="s">
         <v>257</v>
@@ -15996,7 +15996,7 @@
         <v>0.225467758820564</v>
       </c>
     </row>
-    <row r="163" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B163" s="6"/>
       <c r="C163" s="6" t="s">
         <v>259</v>
@@ -16098,7 +16098,7 @@
         <v>71742.123753789405</v>
       </c>
     </row>
-    <row r="164" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B164" s="6"/>
       <c r="C164" s="6" t="s">
         <v>260</v>
@@ -16200,7 +16200,7 @@
         <v>35921.280000000006</v>
       </c>
     </row>
-    <row r="165" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B165" s="6"/>
       <c r="C165" s="6" t="s">
         <v>261</v>
@@ -16302,7 +16302,7 @@
         <v>16733.080000000002</v>
       </c>
     </row>
-    <row r="166" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="166" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B166" s="6"/>
       <c r="C166" s="6" t="s">
         <v>262</v>
@@ -16404,7 +16404,7 @@
         <v>7793.93</v>
       </c>
     </row>
-    <row r="167" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="167" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B167" s="6"/>
       <c r="C167" s="6" t="s">
         <v>263</v>
@@ -16506,7 +16506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="168" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B168" s="6"/>
       <c r="C168" s="6" t="s">
         <v>181</v>
@@ -16608,7 +16608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B169" s="6"/>
       <c r="C169" s="6" t="s">
         <v>264</v>
@@ -16710,7 +16710,7 @@
         <v>5205.13</v>
       </c>
     </row>
-    <row r="170" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="170" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B170" s="6"/>
       <c r="C170" s="6" t="s">
         <v>180</v>
@@ -16812,7 +16812,7 @@
         <v>630.66999999999996</v>
       </c>
     </row>
-    <row r="171" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="171" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B171" s="6"/>
       <c r="C171" s="6" t="s">
         <v>182</v>
@@ -16914,7 +16914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="172" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B172" s="6"/>
       <c r="C172" s="6" t="s">
         <v>159</v>
@@ -17016,7 +17016,7 @@
         <v>2202.1999999999998</v>
       </c>
     </row>
-    <row r="173" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="173" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B173" s="6"/>
       <c r="C173" s="6" t="s">
         <v>158</v>
@@ -17118,7 +17118,7 @@
         <v>720.16</v>
       </c>
     </row>
-    <row r="174" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B174" s="6"/>
       <c r="C174" s="6" t="s">
         <v>168</v>
@@ -17220,7 +17220,7 @@
         <v>2636.1099999999997</v>
       </c>
     </row>
-    <row r="175" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="175" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B175" s="6"/>
       <c r="C175" s="6" t="s">
         <v>265</v>
@@ -17322,7 +17322,7 @@
         <v>-2577.52</v>
       </c>
     </row>
-    <row r="176" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="176" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B176" s="6"/>
       <c r="C176" s="6" t="s">
         <v>266</v>
@@ -17400,7 +17400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="177" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B177" s="6"/>
       <c r="C177" s="6" t="s">
         <v>267</v>
@@ -17502,7 +17502,7 @@
         <v>24380.48</v>
       </c>
     </row>
-    <row r="178" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="178" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B178" s="6"/>
       <c r="C178" s="6" t="s">
         <v>268</v>
@@ -17604,7 +17604,7 @@
         <v>21481.7</v>
       </c>
     </row>
-    <row r="179" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="179" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B179" s="6"/>
       <c r="C179" s="6" t="s">
         <v>167</v>
@@ -17706,7 +17706,7 @@
         <v>2898.7799999999997</v>
       </c>
     </row>
-    <row r="180" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="180" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B180" s="6"/>
       <c r="C180" s="6" t="s">
         <v>269</v>
@@ -17808,7 +17808,7 @@
         <v>11440.37</v>
       </c>
     </row>
-    <row r="181" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="181" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B181" s="6"/>
       <c r="C181" s="6" t="s">
         <v>270</v>
@@ -17910,7 +17910,7 @@
         <v>69164.61</v>
       </c>
     </row>
-    <row r="182" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="182" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B182" s="6"/>
       <c r="C182" s="6" t="s">
         <v>271</v>
@@ -18012,7 +18012,7 @@
         <v>0.22546786949176423</v>
       </c>
     </row>
-    <row r="183" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="183" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B183" s="6"/>
       <c r="C183" s="6" t="s">
         <v>272</v>
@@ -18114,7 +18114,7 @@
         <v>74.562080000000009</v>
       </c>
     </row>
-    <row r="184" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="184" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B184" s="6"/>
       <c r="C184" s="6" t="s">
         <v>274</v>
@@ -18216,7 +18216,7 @@
         <v>1.4985495629604563E-2</v>
       </c>
     </row>
-    <row r="185" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="185" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B185" s="6"/>
       <c r="C185" s="6" t="s">
         <v>275</v>
@@ -18318,7 +18318,7 @@
         <v>0.24956138789331481</v>
       </c>
     </row>
-    <row r="186" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="186" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B186" s="6"/>
       <c r="C186" s="6" t="s">
         <v>276</v>
@@ -18420,22 +18420,22 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="187" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="187" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B187" s="6"/>
     </row>
-    <row r="188" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="188" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B188" s="6"/>
     </row>
-    <row r="189" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="189" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B189" s="6"/>
       <c r="C189" s="6" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="190" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="190" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B190" s="6"/>
     </row>
-    <row r="191" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="191" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B191" s="6"/>
       <c r="D191" t="s">
         <v>136</v>
@@ -18534,7 +18534,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="192" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="192" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B192" s="6"/>
       <c r="C192" s="6" t="s">
         <v>278</v>
@@ -18636,7 +18636,7 @@
         <v>15309.220000000001</v>
       </c>
     </row>
-    <row r="193" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="193" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B193" s="6"/>
       <c r="C193" s="6" t="s">
         <v>279</v>
@@ -18738,16 +18738,16 @@
         <v>304.94043123999995</v>
       </c>
     </row>
-    <row r="194" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="194" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B194" s="6"/>
     </row>
-    <row r="195" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="195" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B195" s="6"/>
       <c r="C195" s="6" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="196" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="196" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B196" s="6"/>
       <c r="C196" s="6" t="s">
         <v>281</v>
@@ -18849,7 +18849,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="197" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="197" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B197" s="6"/>
       <c r="C197" s="6" t="s">
         <v>158</v>
@@ -18951,7 +18951,7 @@
         <v>134.38999999999999</v>
       </c>
     </row>
-    <row r="198" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="198" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B198" s="6"/>
       <c r="C198" s="6" t="s">
         <v>159</v>
@@ -19053,7 +19053,7 @@
         <v>1521.41</v>
       </c>
     </row>
-    <row r="199" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="199" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B199" s="6"/>
       <c r="C199" s="6" t="s">
         <v>164</v>
@@ -19155,7 +19155,7 @@
         <v>72215.049999999988</v>
       </c>
     </row>
-    <row r="200" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="200" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B200" s="6"/>
       <c r="C200" s="6" t="s">
         <v>161</v>
@@ -19257,7 +19257,7 @@
         <v>5031.2699999999995</v>
       </c>
     </row>
-    <row r="201" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="201" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B201" s="6"/>
       <c r="C201" s="6" t="s">
         <v>162</v>
@@ -19359,7 +19359,7 @@
         <v>1970.2</v>
       </c>
     </row>
-    <row r="202" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="202" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B202" s="6"/>
       <c r="C202" s="6" t="s">
         <v>282</v>
@@ -19461,16 +19461,16 @@
         <v>1728.08</v>
       </c>
     </row>
-    <row r="203" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="203" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B203" s="6"/>
     </row>
-    <row r="204" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="204" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B204" s="6"/>
       <c r="C204" s="6" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="205" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="205" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B205" s="6"/>
       <c r="C205" s="6" t="s">
         <v>281</v>
@@ -19572,7 +19572,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="206" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="206" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B206" s="6"/>
       <c r="C206" s="6" t="s">
         <v>159</v>
@@ -19674,7 +19674,7 @@
         <v>1159.71</v>
       </c>
     </row>
-    <row r="207" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="207" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B207" s="6"/>
       <c r="C207" s="6" t="s">
         <v>164</v>
@@ -19776,7 +19776,7 @@
         <v>430.68</v>
       </c>
     </row>
-    <row r="208" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="208" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B208" s="6"/>
       <c r="C208" s="6" t="s">
         <v>161</v>
@@ -19878,7 +19878,7 @@
         <v>949.95</v>
       </c>
     </row>
-    <row r="209" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="209" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B209" s="6"/>
       <c r="C209" s="6" t="s">
         <v>162</v>
@@ -19980,7 +19980,7 @@
         <v>1970.2</v>
       </c>
     </row>
-    <row r="210" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="210" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B210" s="6"/>
       <c r="C210" s="6" t="s">
         <v>282</v>
@@ -20082,16 +20082,16 @@
         <v>1728.08</v>
       </c>
     </row>
-    <row r="211" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="211" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B211" s="6"/>
     </row>
-    <row r="212" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="212" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B212" s="6"/>
       <c r="C212" s="6" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="213" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="213" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B213" s="6"/>
       <c r="C213" s="6" t="s">
         <v>281</v>
@@ -20193,7 +20193,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="214" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="214" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B214" s="6"/>
       <c r="C214" s="6" t="s">
         <v>159</v>
@@ -20295,7 +20295,7 @@
         <v>361.7</v>
       </c>
     </row>
-    <row r="215" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="215" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B215" s="6"/>
       <c r="C215" s="6" t="s">
         <v>164</v>
@@ -20397,7 +20397,7 @@
         <v>71784.37</v>
       </c>
     </row>
-    <row r="216" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="216" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B216" s="6"/>
       <c r="C216" s="6" t="s">
         <v>161</v>
@@ -20499,7 +20499,7 @@
         <v>4081.3199999999997</v>
       </c>
     </row>
-    <row r="217" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="217" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B217" s="6"/>
       <c r="C217" s="6" t="s">
         <v>162</v>
@@ -20601,7 +20601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="218" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B218" s="6"/>
       <c r="C218" s="6" t="s">
         <v>282</v>
@@ -20703,22 +20703,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="219" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B219" s="6"/>
     </row>
-    <row r="220" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="220" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B220" s="6"/>
     </row>
-    <row r="221" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="221" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B221" s="6"/>
       <c r="C221" s="6" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="222" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="222" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B222" s="6"/>
     </row>
-    <row r="223" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="223" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B223" s="6"/>
       <c r="D223" t="s">
         <v>136</v>
@@ -20817,7 +20817,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="224" spans="2:36" x14ac:dyDescent="0.35">
+    <row r="224" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B224" s="6"/>
       <c r="C224" s="6" t="s">
         <v>286</v>
@@ -20929,28 +20929,28 @@
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.26953125" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="10" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="25" max="28" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="30" max="33" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="28" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="33" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>126</v>
       </c>
@@ -20958,13 +20958,13 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:34" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:34" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>287</v>
       </c>
@@ -20972,9 +20972,9 @@
         <v>288</v>
       </c>
     </row>
-    <row r="5" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6" t="s">
         <v>136</v>
@@ -21074,7 +21074,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>166</v>
       </c>
@@ -21207,7 +21207,7 @@
         <v>45277.38</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>2022</v>
       </c>
@@ -21242,7 +21242,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>290</v>
       </c>
@@ -21291,7 +21291,7 @@
         <v>45277.38</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>2022</v>
       </c>
@@ -21380,7 +21380,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>121</v>
       </c>
@@ -21515,15 +21515,15 @@
       <selection sqref="A1:AI1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.26953125" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="32" width="13.7265625" style="19" bestFit="1" customWidth="1"/>
-    <col min="33" max="35" width="15.453125" style="19" bestFit="1" customWidth="1"/>
-    <col min="36" max="16384" width="9.1796875" style="19"/>
+    <col min="1" max="1" width="34.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="32" width="13.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="33" max="35" width="15.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>293</v>
       </c>
@@ -21562,7 +21562,7 @@
       <c r="AH1" s="31"/>
       <c r="AI1" s="31"/>
     </row>
-    <row r="2" spans="1:35" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
@@ -21601,7 +21601,7 @@
       <c r="AH2" s="31"/>
       <c r="AI2" s="31"/>
     </row>
-    <row r="3" spans="1:35" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>294</v>
       </c>
@@ -21640,7 +21640,7 @@
       <c r="AH3" s="32"/>
       <c r="AI3" s="32"/>
     </row>
-    <row r="4" spans="1:35" ht="26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>295</v>
       </c>
@@ -21747,7 +21747,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>330</v>
       </c>
@@ -21854,7 +21854,7 @@
         <v>36.4</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>331</v>
       </c>
@@ -21961,7 +21961,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>159</v>
       </c>
@@ -22068,7 +22068,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>333</v>
       </c>
@@ -22175,7 +22175,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>334</v>
       </c>
@@ -22282,7 +22282,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>335</v>
       </c>
@@ -22389,7 +22389,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>336</v>
       </c>
@@ -22496,7 +22496,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>337</v>
       </c>
@@ -22603,7 +22603,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>338</v>
       </c>
@@ -22710,7 +22710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>339</v>
       </c>
@@ -22817,7 +22817,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>180</v>
       </c>
@@ -22924,7 +22924,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>340</v>
       </c>
@@ -23031,7 +23031,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>341</v>
       </c>
@@ -23138,7 +23138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>342</v>
       </c>
@@ -23245,7 +23245,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>343</v>
       </c>
@@ -23352,7 +23352,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>344</v>
       </c>
@@ -23459,7 +23459,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
         <v>345</v>
       </c>
@@ -23566,7 +23566,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>164</v>
       </c>
@@ -23673,7 +23673,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>346</v>
       </c>
@@ -23780,7 +23780,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
         <v>161</v>
       </c>
@@ -23887,7 +23887,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
         <v>347</v>
       </c>
@@ -23994,7 +23994,7 @@
         <v>63.6</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
         <v>331</v>
       </c>
@@ -24101,7 +24101,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>182</v>
       </c>
@@ -24208,7 +24208,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
         <v>159</v>
       </c>
@@ -24315,7 +24315,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
         <v>333</v>
       </c>
@@ -24422,7 +24422,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
         <v>334</v>
       </c>
@@ -24529,7 +24529,7 @@
         <v>32.6</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
         <v>335</v>
       </c>
@@ -24636,7 +24636,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>336</v>
       </c>
@@ -24743,7 +24743,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>337</v>
       </c>
@@ -24850,7 +24850,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>338</v>
       </c>
@@ -24957,7 +24957,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>339</v>
       </c>
@@ -25064,7 +25064,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
         <v>340</v>
       </c>
@@ -25171,7 +25171,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
         <v>341</v>
       </c>
@@ -25278,7 +25278,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
         <v>348</v>
       </c>
@@ -25385,7 +25385,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>342</v>
       </c>
@@ -25492,7 +25492,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>343</v>
       </c>
@@ -25599,7 +25599,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
         <v>344</v>
       </c>
@@ -25706,7 +25706,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
         <v>349</v>
       </c>
@@ -25813,7 +25813,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
         <v>350</v>
       </c>
@@ -25920,7 +25920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
         <v>345</v>
       </c>
@@ -26027,7 +26027,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45" s="23" t="s">
         <v>164</v>
       </c>
@@ -26134,7 +26134,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
         <v>346</v>
       </c>
@@ -26241,7 +26241,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47" s="25" t="s">
         <v>351</v>
       </c>
@@ -26348,7 +26348,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48" s="23" t="s">
         <v>161</v>
       </c>
@@ -26455,7 +26455,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49" s="23" t="s">
         <v>352</v>
       </c>
@@ -26562,7 +26562,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
         <v>353</v>
       </c>
@@ -26669,7 +26669,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51" s="23" t="s">
         <v>331</v>
       </c>
@@ -26776,7 +26776,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52" s="23" t="s">
         <v>182</v>
       </c>
@@ -26883,7 +26883,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
         <v>159</v>
       </c>
@@ -26990,7 +26990,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54" s="23" t="s">
         <v>333</v>
       </c>
@@ -27097,7 +27097,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55" s="23" t="s">
         <v>334</v>
       </c>
@@ -27204,7 +27204,7 @@
         <v>47.4</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56" s="25" t="s">
         <v>335</v>
       </c>
@@ -27311,7 +27311,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57" s="25" t="s">
         <v>336</v>
       </c>
@@ -27418,7 +27418,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58" s="25" t="s">
         <v>337</v>
       </c>
@@ -27525,7 +27525,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59" s="25" t="s">
         <v>338</v>
       </c>
@@ -27632,7 +27632,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60" s="25" t="s">
         <v>339</v>
       </c>
@@ -27739,7 +27739,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61" s="23" t="s">
         <v>180</v>
       </c>
@@ -27846,7 +27846,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62" s="23" t="s">
         <v>340</v>
       </c>
@@ -27953,7 +27953,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63" s="23" t="s">
         <v>341</v>
       </c>
@@ -28060,7 +28060,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64" s="23" t="s">
         <v>348</v>
       </c>
@@ -28167,7 +28167,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65" s="23" t="s">
         <v>342</v>
       </c>
@@ -28274,7 +28274,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66" s="25" t="s">
         <v>343</v>
       </c>
@@ -28381,7 +28381,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A67" s="25" t="s">
         <v>344</v>
       </c>
@@ -28488,7 +28488,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A68" s="25" t="s">
         <v>349</v>
       </c>
@@ -28595,7 +28595,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A69" s="25" t="s">
         <v>350</v>
       </c>
@@ -28702,7 +28702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A70" s="23" t="s">
         <v>345</v>
       </c>
@@ -28809,7 +28809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A71" s="23" t="s">
         <v>164</v>
       </c>
@@ -28916,7 +28916,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A72" s="25" t="s">
         <v>346</v>
       </c>
@@ -29023,7 +29023,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="73" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A73" s="25" t="s">
         <v>351</v>
       </c>
@@ -29130,7 +29130,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="74" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A74" s="23" t="s">
         <v>161</v>
       </c>
@@ -29237,7 +29237,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A75" s="23" t="s">
         <v>352</v>
       </c>
@@ -29344,7 +29344,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="76" spans="1:35" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:35" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="33" t="s">
         <v>354</v>
       </c>
@@ -29405,13 +29405,13 @@
       <selection activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.1796875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" style="6" customWidth="1"/>
     <col min="2" max="2" width="9" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>123</v>
       </c>
@@ -29512,7 +29512,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -29659,17 +29659,17 @@
   <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="AG3" sqref="AG3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.1796875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="33" width="10.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="33" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>123</v>
       </c>
@@ -29770,137 +29770,133 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>124</v>
       </c>
       <c r="B2" s="17">
-        <f>BGBSC!B2</f>
-        <v>252.5</v>
+        <v>0</v>
       </c>
       <c r="C2" s="17">
-        <f>BGBSC!C2</f>
-        <v>524.29999999999995</v>
+        <v>0</v>
       </c>
       <c r="D2" s="17">
-        <f>BGBSC!D2</f>
-        <v>2842.27</v>
+        <v>0</v>
       </c>
       <c r="E2" s="17">
-        <f>BGBSC!E2</f>
-        <v>5160.24</v>
+        <v>0</v>
       </c>
       <c r="F2" s="17">
-        <f>BGBSC!F2</f>
-        <v>7563.37</v>
+        <f>$AG$2/COUNT($F$1:$AG$1)+E2</f>
+        <v>512.9920535714233</v>
       </c>
       <c r="G2" s="17">
-        <f>BGBSC!G2</f>
-        <v>13055.18</v>
+        <f t="shared" ref="G2:AF2" si="0">$AG$2/COUNT($F$1:$AG$1)+F2</f>
+        <v>1025.9841071428466</v>
       </c>
       <c r="H2" s="17">
-        <f>BGBSC!H2</f>
-        <v>14769.37</v>
+        <f t="shared" si="0"/>
+        <v>1538.97616071427</v>
       </c>
       <c r="I2" s="17">
-        <f>BGBSC!I2</f>
-        <v>14983.48</v>
+        <f t="shared" si="0"/>
+        <v>2051.9682142856932</v>
       </c>
       <c r="J2" s="17">
-        <f>BGBSC!J2</f>
-        <v>15585.665000000037</v>
+        <f t="shared" si="0"/>
+        <v>2564.9602678571164</v>
       </c>
       <c r="K2" s="17">
-        <f>BGBSC!K2</f>
-        <v>16187.849999999999</v>
+        <f t="shared" si="0"/>
+        <v>3077.9523214285396</v>
       </c>
       <c r="L2" s="17">
-        <f>BGBSC!L2</f>
-        <v>16576.844999999972</v>
+        <f t="shared" si="0"/>
+        <v>3590.9443749999627</v>
       </c>
       <c r="M2" s="17">
-        <f>BGBSC!M2</f>
-        <v>16965.84</v>
+        <f t="shared" si="0"/>
+        <v>4103.9364285713864</v>
       </c>
       <c r="N2" s="17">
-        <f>BGBSC!N2</f>
-        <v>17553.909999999916</v>
+        <f t="shared" si="0"/>
+        <v>4616.92848214281</v>
       </c>
       <c r="O2" s="17">
-        <f>BGBSC!O2</f>
-        <v>18141.98</v>
+        <f t="shared" si="0"/>
+        <v>5129.9205357142337</v>
       </c>
       <c r="P2" s="17">
-        <f>BGBSC!P2</f>
-        <v>19501.040000000037</v>
+        <f t="shared" si="0"/>
+        <v>5642.9125892856573</v>
       </c>
       <c r="Q2" s="17">
-        <f>BGBSC!Q2</f>
-        <v>20860.100000000093</v>
+        <f t="shared" si="0"/>
+        <v>6155.9046428570809</v>
       </c>
       <c r="R2" s="17">
-        <f>BGBSC!R2</f>
-        <v>22219.159999999996</v>
+        <f t="shared" si="0"/>
+        <v>6668.8966964285046</v>
       </c>
       <c r="S2" s="17">
-        <f>BGBSC!S2</f>
-        <v>24395.25800000038</v>
+        <f t="shared" si="0"/>
+        <v>7181.8887499999282</v>
       </c>
       <c r="T2" s="17">
-        <f>BGBSC!T2</f>
-        <v>26571.356000000611</v>
+        <f t="shared" si="0"/>
+        <v>7694.8808035713519</v>
       </c>
       <c r="U2" s="17">
-        <f>BGBSC!U2</f>
-        <v>28747.453999999911</v>
+        <f t="shared" si="0"/>
+        <v>8207.8728571427746</v>
       </c>
       <c r="V2" s="17">
-        <f>BGBSC!V2</f>
-        <v>30923.552000000142</v>
+        <f t="shared" si="0"/>
+        <v>8720.8649107141973</v>
       </c>
       <c r="W2" s="17">
-        <f>BGBSC!W2</f>
-        <v>33099.650000000373</v>
+        <f t="shared" si="0"/>
+        <v>9233.8569642856201</v>
       </c>
       <c r="X2" s="17">
-        <f>BGBSC!X2</f>
-        <v>35535.195999999531</v>
+        <f t="shared" si="0"/>
+        <v>9746.8490178570428</v>
       </c>
       <c r="Y2" s="17">
-        <f>BGBSC!Y2</f>
-        <v>37970.74199999962</v>
+        <f t="shared" si="0"/>
+        <v>10259.841071428466</v>
       </c>
       <c r="Z2" s="17">
-        <f>BGBSC!Z2</f>
-        <v>40406.287999998778</v>
+        <f t="shared" si="0"/>
+        <v>10772.833124999888</v>
       </c>
       <c r="AA2" s="17">
-        <f>BGBSC!AA2</f>
-        <v>42841.833999998868</v>
+        <f t="shared" si="0"/>
+        <v>11285.825178571311</v>
       </c>
       <c r="AB2" s="17">
-        <f>BGBSC!AB2</f>
-        <v>45277.379999998957</v>
+        <f t="shared" si="0"/>
+        <v>11798.817232142734</v>
       </c>
       <c r="AC2" s="17">
-        <f>BGBSC!AC2</f>
-        <v>47712.925999999046</v>
+        <f t="shared" si="0"/>
+        <v>12311.809285714156</v>
       </c>
       <c r="AD2" s="17">
-        <f>BGBSC!AD2</f>
-        <v>50148.471999999136</v>
+        <f t="shared" si="0"/>
+        <v>12824.801339285579</v>
       </c>
       <c r="AE2" s="17">
-        <f>BGBSC!AE2</f>
-        <v>52584.017999999225</v>
+        <f t="shared" si="0"/>
+        <v>13337.793392857002</v>
       </c>
       <c r="AF2" s="17">
-        <f>BGBSC!AF2</f>
-        <v>55019.563999999315</v>
+        <f t="shared" si="0"/>
+        <v>13850.785446428425</v>
       </c>
       <c r="AG2" s="17">
-        <f>BGBSC!AG2</f>
-        <v>57455.109999999404</v>
+        <f>BGBSC!AG2*0.25</f>
+        <v>14363.777499999851</v>
       </c>
     </row>
   </sheetData>
@@ -29920,15 +29916,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="9.1796875" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="6"/>
+    <col min="1" max="1" width="11.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>123</v>
       </c>
@@ -29936,7 +29932,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -29945,7 +29941,7 @@
         <v>252.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
     </row>
   </sheetData>

</xml_diff>